<commit_message>
Update docs, validation logic, and gitignore
</commit_message>
<xml_diff>
--- a/template_extracted_studies.xlsx
+++ b/template_extracted_studies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:AS1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,211 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Study ID</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Country/Region</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Study Design</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Database/Setting</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Age (mean ± SD)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Sample Size (Total)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>GLP-1 RA Cohort Size</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Control cohort Size</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Sex (% male/female)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Diabetes Status (%)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Obesity/BMI (mean or %)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Smoking History (%)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Comorbidities</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Indication for Spine Surgery</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Surgical Procedure</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Levels of Surgery</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Follow-up Duration</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Bone Mineral Density (BMD)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Glycemic Control (HbA1c)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Glucagon-like peptide-1 receptor agonist Details</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Preoperative GLP-1 RA exposure duration</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Control Group Details</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Primary Outcome(s)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Secondary Outcome(s)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Intraoperative Complications</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Postoperative Complications</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Surgical Site Infection (SSI)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Reoperation Rates</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Pseudoarthrosis/Fusion Failure</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Readmission</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Mortality</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Other Medical Complications</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Blood Loss</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Operative Time</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Hospital Length of Stay (LOS)</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Patient-Reported Outcomes (PROMs)</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Cost/Economic Analysis</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Key Findings/Conclusion</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Subgroup Analysis</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Heterogeneity</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Risk of Bias/Quality Assessment</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
           <t>Source File</t>
         </is>
       </c>

</xml_diff>